<commit_message>
Update Kho gửi phòng SX-BH 02_2026.xlsx
</commit_message>
<xml_diff>
--- a/5. Other/Thiết bị kho gửi/2026/Kho gửi phòng SX-BH 02_2026.xlsx
+++ b/5. Other/Thiết bị kho gửi/2026/Kho gửi phòng SX-BH 02_2026.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNET\5. Other\Thiết bị kho gửi\2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1966EE7B-0405-48EC-A1B9-525742278291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D9B73C-2946-46D5-9DC2-7A844EB93492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nhập xuất tồn" sheetId="1" r:id="rId1"/>
@@ -1222,18 +1222,18 @@
       </c>
       <c r="E4" s="4">
         <f>Xuất!AH5+Huỷ!AH4</f>
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F4" s="4">
         <f>C4+D4-E4</f>
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G4" s="6">
         <v>16</v>
       </c>
       <c r="H4" s="4">
         <f t="shared" ref="H4:H22" si="0">F4-G4</f>
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1798,11 +1798,11 @@
       </c>
       <c r="E23" s="4">
         <f t="shared" si="2"/>
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" si="2"/>
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="2"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="H23" s="4">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1851,7 +1851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH22"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showZeros="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -2868,7 +2868,7 @@
   <dimension ref="A1:AH23"/>
   <sheetViews>
     <sheetView showZeros="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3127,7 +3127,9 @@
       <c r="H5" s="7">
         <v>31</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7">
+        <v>6</v>
+      </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
@@ -3154,7 +3156,7 @@
       <c r="AG5" s="7"/>
       <c r="AH5" s="7">
         <f t="shared" ref="AH5:AH18" si="0">SUM(C5:AG5)</f>
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
@@ -4948,8 +4950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C51F44-131D-46D9-8F20-A11BD47AE60F}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5622,18 +5624,18 @@
       </c>
       <c r="E4" s="4">
         <f>SUM('Nhập xuất tồn'!E4)</f>
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F4" s="4">
         <f>SUM(C4+D4-E4)</f>
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G4" s="6">
         <v>16</v>
       </c>
       <c r="H4" s="4">
         <f>SUM(F4-G4)</f>
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6044,11 +6046,11 @@
       </c>
       <c r="E18" s="12">
         <f t="shared" si="2"/>
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F18" s="12">
         <f t="shared" si="2"/>
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="G18" s="13">
         <f t="shared" ref="G18" si="3">SUM(G3:G17)</f>
@@ -6056,7 +6058,7 @@
       </c>
       <c r="H18" s="12">
         <f t="shared" ref="H18" si="4">SUM(H3:H17)</f>
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>